<commit_message>
Added draft presentation. Updated other docs
</commit_message>
<xml_diff>
--- a/docs/Test cases.xlsx
+++ b/docs/Test cases.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="783" uniqueCount="362">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="783" uniqueCount="361">
   <si>
     <t>ID</t>
   </si>
@@ -265,20 +265,12 @@
     <t>Category name=""</t>
   </si>
   <si>
-    <t xml:space="preserve">A popup appears. On 
-clicking Delete, the category gets deleted.  </t>
-  </si>
-  <si>
     <t>Swipe left or right the created category. Click 'Delete' in the toast that appears on screen.</t>
   </si>
   <si>
     <t>Category name="Red"</t>
   </si>
   <si>
-    <t xml:space="preserve">A popup appears. On 
-clicking Rename, the category gets renamed.  </t>
-  </si>
-  <si>
     <t>A Category is not created</t>
   </si>
   <si>
@@ -297,14 +289,6 @@
     <t>Category name="Blue"</t>
   </si>
   <si>
-    <t>Word gets assigned to
- that category.</t>
-  </si>
-  <si>
-    <t>Word gets assigned to
-that category.</t>
-  </si>
-  <si>
     <t>Assign word to category 'Black'</t>
   </si>
   <si>
@@ -323,10 +307,6 @@
     <t>Assign word to category 'Red' &amp; 'Black'</t>
   </si>
   <si>
-    <t>Word gets assigned to
-multiple category.</t>
-  </si>
-  <si>
     <t>Remove word from all categories</t>
   </si>
   <si>
@@ -334,9 +314,6 @@
   </si>
   <si>
     <t>Deselect all categories.</t>
-  </si>
-  <si>
-    <t>Word not assigned to any category.</t>
   </si>
   <si>
     <t>Search multiple words in vocubalary section. Click 'Filter' button.</t>
@@ -398,9 +375,6 @@
     <t>Select category to filter words with.</t>
   </si>
   <si>
-    <t xml:space="preserve">All Categories populated in the filter list. </t>
-  </si>
-  <si>
     <t>Splash screen</t>
   </si>
   <si>
@@ -416,9 +390,6 @@
     <t>Legal page loads.</t>
   </si>
   <si>
-    <t>Splash screen loads.</t>
-  </si>
-  <si>
     <t>Click Help (?) icon</t>
   </si>
   <si>
@@ -440,10 +411,6 @@
     <t>Search term = "Practical"</t>
   </si>
   <si>
-    <t>Recent words get 
-populated in search history.</t>
-  </si>
-  <si>
     <t>Swipe left or right on the words from recent search history</t>
   </si>
   <si>
@@ -451,10 +418,6 @@
   </si>
   <si>
     <t>Click the 'Copy to clipboard' button</t>
-  </si>
-  <si>
-    <t>A toast appears 
-confirming that all words in the search history list have been copied.</t>
   </si>
   <si>
     <t>Search term=""</t>
@@ -491,18 +454,10 @@
     <t>Search term="Theory"</t>
   </si>
   <si>
-    <t>A card with word 
-definition appears &amp; the word doesn’t get populated again.</t>
-  </si>
-  <si>
     <t>No category with same name</t>
   </si>
   <si>
     <t>Create a new category with already existing name</t>
-  </si>
-  <si>
-    <t>A toast appears saying 
-Category already exists.</t>
   </si>
   <si>
     <t>Create a new category with already existing name with Caps ON</t>
@@ -540,23 +495,10 @@
     <t>New email="brahmpreet.official@gmail.com", Current password="12"</t>
   </si>
   <si>
-    <t>Email not updated. 
-Toast with error.</t>
-  </si>
-  <si>
     <t>Current password="12345", New password="56789",
  Repeat Password="56789"</t>
   </si>
   <si>
-    <t>Password changed.</t>
-  </si>
-  <si>
-    <t>Logged out of app session.</t>
-  </si>
-  <si>
-    <t>Account deleted.</t>
-  </si>
-  <si>
     <t>Click settings icon. Select 'Logout'.</t>
   </si>
   <si>
@@ -790,17 +732,7 @@
     <t>Click microphone button in the vocabulary section. Speak the word to be searched.</t>
   </si>
   <si>
-    <t>Spoken word appears in 
-search term.</t>
-  </si>
-  <si>
-    <t>Scanned word appear in Search.</t>
-  </si>
-  <si>
     <t>UI interface</t>
-  </si>
-  <si>
-    <t>The list is scrollable.</t>
   </si>
   <si>
     <t>Final score calculated is
@@ -828,9 +760,6 @@
 textfield</t>
   </si>
   <si>
-    <t>App reads the text aloud.</t>
-  </si>
-  <si>
     <t xml:space="preserve">UI interface </t>
   </si>
   <si>
@@ -842,9 +771,6 @@
   </si>
   <si>
     <t>Camera</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Click camera button in the the vocubalary section. </t>
   </si>
   <si>
     <t>Storage</t>
@@ -1229,6 +1155,77 @@
   </si>
   <si>
     <t>Button not clicked outside bounds</t>
+  </si>
+  <si>
+    <t>Splash screen loads</t>
+  </si>
+  <si>
+    <t>Word gets assigned to
+that category</t>
+  </si>
+  <si>
+    <t>Word gets assigned to
+multiple category</t>
+  </si>
+  <si>
+    <t>Word gets assigned to
+ that category</t>
+  </si>
+  <si>
+    <t>Word not assigned to any category</t>
+  </si>
+  <si>
+    <t>All Categories populated in the filter list</t>
+  </si>
+  <si>
+    <t>Recent words get 
+populated in search history</t>
+  </si>
+  <si>
+    <t>A popup appears. On 
+clicking Rename, the category gets renamed</t>
+  </si>
+  <si>
+    <t>A popup appears. On 
+clicking Delete, the category gets deleted</t>
+  </si>
+  <si>
+    <t>A toast appears saying 
+Category already exists</t>
+  </si>
+  <si>
+    <t>A toast appears 
+confirming that all words in the search history list have been copied</t>
+  </si>
+  <si>
+    <t>A card with word 
+definition appears &amp; the word doesn’t get populated again</t>
+  </si>
+  <si>
+    <t>Password changed</t>
+  </si>
+  <si>
+    <t>Email not updated. 
+Toast with error shown</t>
+  </si>
+  <si>
+    <t>Logged out of app session</t>
+  </si>
+  <si>
+    <t>Account deleted</t>
+  </si>
+  <si>
+    <t>Scanned word appear in Search</t>
+  </si>
+  <si>
+    <t>Spoken word appears in 
+search field</t>
+  </si>
+  <si>
+    <t>App reads the text aloud</t>
+  </si>
+  <si>
+    <t>Click camera button in the the vocubalary section</t>
   </si>
 </sst>
 </file>
@@ -1640,8 +1637,8 @@
   <dimension ref="A1:I109"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A73" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D110" sqref="D110"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1691,21 +1688,21 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>278</v>
+        <v>257</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4" t="s">
-        <v>290</v>
+        <v>269</v>
       </c>
       <c r="F2" s="4"/>
       <c r="G2" s="4" t="s">
-        <v>105</v>
+        <v>341</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>105</v>
+        <v>341</v>
       </c>
       <c r="I2" s="4" t="s">
         <v>11</v>
@@ -1716,21 +1713,21 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>314</v>
+        <v>293</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>315</v>
+        <v>294</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="4" t="s">
-        <v>290</v>
+        <v>269</v>
       </c>
       <c r="F3" s="4"/>
       <c r="G3" s="4" t="s">
-        <v>164</v>
+        <v>148</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>165</v>
+        <v>149</v>
       </c>
       <c r="I3" s="4" t="s">
         <v>11</v>
@@ -1747,7 +1744,7 @@
         <v>14</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>345</v>
+        <v>324</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>29</v>
@@ -1773,13 +1770,13 @@
         <v>36</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>241</v>
+        <v>220</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>345</v>
+        <v>324</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>242</v>
+        <v>221</v>
       </c>
       <c r="F5" s="4" t="s">
         <v>38</v>
@@ -1802,22 +1799,22 @@
         <v>36</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>243</v>
+        <v>222</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>345</v>
+        <v>324</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>242</v>
+        <v>221</v>
       </c>
       <c r="F6" s="4" t="s">
         <v>39</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>245</v>
+        <v>224</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>245</v>
+        <v>224</v>
       </c>
       <c r="I6" s="3" t="s">
         <v>11</v>
@@ -1831,10 +1828,10 @@
         <v>36</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>244</v>
+        <v>223</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>345</v>
+        <v>324</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>30</v>
@@ -1863,10 +1860,10 @@
         <v>16</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>345</v>
+        <v>324</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>246</v>
+        <v>225</v>
       </c>
       <c r="F8" s="4" t="s">
         <v>41</v>
@@ -1892,7 +1889,7 @@
         <v>23</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>344</v>
+        <v>323</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>31</v>
@@ -1921,10 +1918,10 @@
         <v>21</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>345</v>
+        <v>324</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>247</v>
+        <v>226</v>
       </c>
       <c r="F10" s="4" t="s">
         <v>43</v>
@@ -1950,7 +1947,7 @@
         <v>14</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>267</v>
+        <v>246</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>12</v>
@@ -1979,7 +1976,7 @@
         <v>15</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>267</v>
+        <v>246</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>13</v>
@@ -1988,10 +1985,10 @@
         <v>26</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>248</v>
+        <v>227</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>248</v>
+        <v>227</v>
       </c>
       <c r="I12" s="4" t="s">
         <v>11</v>
@@ -2008,7 +2005,7 @@
         <v>28</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>267</v>
+        <v>246</v>
       </c>
       <c r="E13" s="4" t="s">
         <v>13</v>
@@ -2037,7 +2034,7 @@
         <v>16</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>267</v>
+        <v>246</v>
       </c>
       <c r="E14" s="4" t="s">
         <v>20</v>
@@ -2066,7 +2063,7 @@
         <v>21</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>267</v>
+        <v>246</v>
       </c>
       <c r="E15" s="4" t="s">
         <v>22</v>
@@ -2095,7 +2092,7 @@
         <v>23</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>267</v>
+        <v>246</v>
       </c>
       <c r="E16" s="4" t="s">
         <v>24</v>
@@ -2104,10 +2101,10 @@
         <v>34</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>248</v>
+        <v>227</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>248</v>
+        <v>227</v>
       </c>
       <c r="I16" s="4" t="s">
         <v>11</v>
@@ -2124,13 +2121,13 @@
         <v>14</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>267</v>
+        <v>246</v>
       </c>
       <c r="E17" s="4" t="s">
         <v>45</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>252</v>
+        <v>231</v>
       </c>
       <c r="G17" s="4" t="s">
         <v>10</v>
@@ -2153,13 +2150,13 @@
         <v>15</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>267</v>
+        <v>246</v>
       </c>
       <c r="E18" s="4" t="s">
         <v>46</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>251</v>
+        <v>230</v>
       </c>
       <c r="G18" s="4" t="s">
         <v>10</v>
@@ -2179,13 +2176,13 @@
         <v>42</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>249</v>
+        <v>228</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>267</v>
+        <v>246</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>250</v>
+        <v>229</v>
       </c>
       <c r="F19" s="4" t="s">
         <v>47</v>
@@ -2211,13 +2208,13 @@
         <v>44</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>267</v>
+        <v>246</v>
       </c>
       <c r="E20" s="4" t="s">
         <v>48</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>253</v>
+        <v>232</v>
       </c>
       <c r="G20" s="4" t="s">
         <v>10</v>
@@ -2240,7 +2237,7 @@
         <v>23</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>267</v>
+        <v>246</v>
       </c>
       <c r="E21" s="4" t="s">
         <v>46</v>
@@ -2266,10 +2263,10 @@
         <v>42</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>254</v>
+        <v>233</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>267</v>
+        <v>246</v>
       </c>
       <c r="E22" s="4" t="s">
         <v>50</v>
@@ -2292,25 +2289,25 @@
         <v>22</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>346</v>
+        <v>325</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>255</v>
+        <v>234</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="H23" s="4" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="I23" s="4" t="s">
         <v>11</v>
@@ -2321,25 +2318,25 @@
         <v>23</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>346</v>
+        <v>325</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>56</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>256</v>
+        <v>235</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>270</v>
+        <v>249</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>70</v>
+        <v>342</v>
       </c>
       <c r="H24" s="4" t="s">
-        <v>69</v>
+        <v>344</v>
       </c>
       <c r="I24" s="4" t="s">
         <v>11</v>
@@ -2350,25 +2347,25 @@
         <v>24</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>346</v>
+        <v>325</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>271</v>
+        <v>250</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>70</v>
+        <v>342</v>
       </c>
       <c r="H25" s="4" t="s">
-        <v>70</v>
+        <v>342</v>
       </c>
       <c r="I25" s="4" t="s">
         <v>11</v>
@@ -2379,25 +2376,25 @@
         <v>25</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>346</v>
+        <v>325</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>272</v>
+        <v>251</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>273</v>
+        <v>252</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>77</v>
+        <v>343</v>
       </c>
       <c r="H26" s="4" t="s">
-        <v>77</v>
+        <v>343</v>
       </c>
       <c r="I26" s="4" t="s">
         <v>11</v>
@@ -2408,25 +2405,25 @@
         <v>26</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>346</v>
+        <v>325</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>274</v>
+        <v>253</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>81</v>
+        <v>345</v>
       </c>
       <c r="H27" s="4" t="s">
-        <v>81</v>
+        <v>345</v>
       </c>
       <c r="I27" s="4" t="s">
         <v>11</v>
@@ -2437,25 +2434,25 @@
         <v>27</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>346</v>
+        <v>325</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>275</v>
+        <v>254</v>
       </c>
       <c r="E28" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="F28" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="F28" s="4" t="s">
-        <v>93</v>
-      </c>
       <c r="G28" s="4" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="H28" s="4" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="I28" s="4" t="s">
         <v>11</v>
@@ -2466,25 +2463,25 @@
         <v>28</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>346</v>
+        <v>325</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>275</v>
+        <v>254</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="G29" s="4" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="H29" s="4" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="I29" s="4" t="s">
         <v>11</v>
@@ -2495,25 +2492,25 @@
         <v>29</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>346</v>
+        <v>325</v>
       </c>
       <c r="C30" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="F30" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="D30" s="4" t="s">
-        <v>275</v>
-      </c>
-      <c r="E30" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="F30" s="4" t="s">
-        <v>95</v>
-      </c>
       <c r="G30" s="4" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="H30" s="4" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="I30" s="4" t="s">
         <v>11</v>
@@ -2524,25 +2521,25 @@
         <v>30</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>346</v>
+        <v>325</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>275</v>
+        <v>254</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="H31" s="4" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="I31" s="4" t="s">
         <v>11</v>
@@ -2553,25 +2550,25 @@
         <v>31</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>346</v>
+        <v>325</v>
       </c>
       <c r="C32" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>235</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="F32" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="D32" s="4" t="s">
-        <v>256</v>
-      </c>
-      <c r="E32" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="F32" s="4" t="s">
-        <v>98</v>
-      </c>
       <c r="G32" s="4" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="H32" s="4" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="I32" s="4" t="s">
         <v>11</v>
@@ -2582,23 +2579,23 @@
         <v>32</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>346</v>
+        <v>325</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>276</v>
+        <v>255</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>256</v>
+        <v>235</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="F33" s="4"/>
       <c r="G33" s="4" t="s">
-        <v>99</v>
+        <v>346</v>
       </c>
       <c r="H33" s="4" t="s">
-        <v>99</v>
+        <v>346</v>
       </c>
       <c r="I33" s="4" t="s">
         <v>11</v>
@@ -2609,25 +2606,25 @@
         <v>33</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>346</v>
+        <v>325</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>255</v>
+        <v>234</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="G34" s="4" t="s">
-        <v>113</v>
+        <v>347</v>
       </c>
       <c r="H34" s="4" t="s">
-        <v>113</v>
+        <v>347</v>
       </c>
       <c r="I34" s="4" t="s">
         <v>11</v>
@@ -2638,23 +2635,23 @@
         <v>34</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>346</v>
+        <v>325</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>279</v>
+        <v>258</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>280</v>
+        <v>259</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="F35" s="4"/>
       <c r="G35" s="4" t="s">
-        <v>281</v>
+        <v>260</v>
       </c>
       <c r="H35" s="4" t="s">
-        <v>281</v>
+        <v>260</v>
       </c>
       <c r="I35" s="4" t="s">
         <v>11</v>
@@ -2665,23 +2662,23 @@
         <v>35</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>346</v>
+        <v>325</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>280</v>
+        <v>259</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="F36" s="4"/>
       <c r="G36" s="4" t="s">
-        <v>117</v>
+        <v>351</v>
       </c>
       <c r="H36" s="4" t="s">
-        <v>117</v>
+        <v>351</v>
       </c>
       <c r="I36" s="4" t="s">
         <v>11</v>
@@ -2692,25 +2689,25 @@
         <v>36</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>346</v>
+        <v>325</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>280</v>
+        <v>259</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="G37" s="4" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="H37" s="4" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="I37" s="4" t="s">
         <v>11</v>
@@ -2721,23 +2718,23 @@
         <v>37</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>346</v>
+        <v>325</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>280</v>
+        <v>259</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="F38" s="4"/>
       <c r="G38" s="4" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="H38" s="4" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="I38" s="4" t="s">
         <v>11</v>
@@ -2748,25 +2745,25 @@
         <v>38</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>346</v>
+        <v>325</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>280</v>
+        <v>259</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="G39" s="4" t="s">
-        <v>128</v>
+        <v>352</v>
       </c>
       <c r="H39" s="4" t="s">
-        <v>128</v>
+        <v>352</v>
       </c>
       <c r="I39" s="4" t="s">
         <v>11</v>
@@ -2783,19 +2780,19 @@
         <v>52</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>255</v>
+        <v>234</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F40" s="4" t="s">
         <v>57</v>
       </c>
       <c r="G40" s="4" t="s">
-        <v>257</v>
+        <v>236</v>
       </c>
       <c r="H40" s="4" t="s">
-        <v>257</v>
+        <v>236</v>
       </c>
       <c r="I40" s="4" t="s">
         <v>11</v>
@@ -2809,13 +2806,13 @@
         <v>51</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>258</v>
+        <v>237</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>255</v>
+        <v>234</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F41" s="4" t="s">
         <v>58</v>
@@ -2838,22 +2835,22 @@
         <v>51</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>259</v>
+        <v>238</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>255</v>
+        <v>234</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F42" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G42" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="H42" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="I42" s="4" t="s">
         <v>11</v>
@@ -2867,22 +2864,22 @@
         <v>51</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>129</v>
+        <v>118</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>255</v>
+        <v>234</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>130</v>
+        <v>119</v>
       </c>
       <c r="F43" s="4" t="s">
         <v>57</v>
       </c>
       <c r="G43" s="4" t="s">
-        <v>131</v>
+        <v>350</v>
       </c>
       <c r="H43" s="4" t="s">
-        <v>131</v>
+        <v>350</v>
       </c>
       <c r="I43" s="4" t="s">
         <v>11</v>
@@ -2896,22 +2893,22 @@
         <v>51</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>277</v>
+        <v>256</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>255</v>
+        <v>234</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>132</v>
+        <v>120</v>
       </c>
       <c r="F44" s="4" t="s">
-        <v>133</v>
+        <v>121</v>
       </c>
       <c r="G44" s="4" t="s">
-        <v>131</v>
+        <v>350</v>
       </c>
       <c r="H44" s="4" t="s">
-        <v>131</v>
+        <v>350</v>
       </c>
       <c r="I44" s="4" t="s">
         <v>11</v>
@@ -2928,17 +2925,17 @@
         <v>53</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>255</v>
+        <v>234</v>
       </c>
       <c r="E45" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F45" s="4"/>
       <c r="G45" s="4" t="s">
-        <v>59</v>
+        <v>349</v>
       </c>
       <c r="H45" s="4" t="s">
-        <v>59</v>
+        <v>349</v>
       </c>
       <c r="I45" s="4" t="s">
         <v>11</v>
@@ -2955,19 +2952,19 @@
         <v>54</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>255</v>
+        <v>234</v>
       </c>
       <c r="E46" s="4" t="s">
-        <v>260</v>
+        <v>239</v>
       </c>
       <c r="F46" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G46" s="4" t="s">
-        <v>62</v>
+        <v>348</v>
       </c>
       <c r="H46" s="4" t="s">
-        <v>62</v>
+        <v>348</v>
       </c>
       <c r="I46" s="4" t="s">
         <v>11</v>
@@ -2981,22 +2978,22 @@
         <v>51</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>262</v>
+        <v>241</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>255</v>
+        <v>234</v>
       </c>
       <c r="E47" s="4" t="s">
-        <v>261</v>
+        <v>240</v>
       </c>
       <c r="F47" s="4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G47" s="4" t="s">
-        <v>265</v>
+        <v>244</v>
       </c>
       <c r="H47" s="4" t="s">
-        <v>265</v>
+        <v>244</v>
       </c>
       <c r="I47" s="4" t="s">
         <v>11</v>
@@ -3010,16 +3007,16 @@
         <v>51</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>263</v>
+        <v>242</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>266</v>
+        <v>245</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>264</v>
+        <v>243</v>
       </c>
       <c r="F48" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G48" s="4" t="s">
         <v>10</v>
@@ -3042,17 +3039,17 @@
         <v>55</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>255</v>
+        <v>234</v>
       </c>
       <c r="E49" s="4" t="s">
-        <v>269</v>
+        <v>248</v>
       </c>
       <c r="F49" s="4"/>
       <c r="G49" s="4" t="s">
-        <v>268</v>
+        <v>247</v>
       </c>
       <c r="H49" s="4" t="s">
-        <v>268</v>
+        <v>247</v>
       </c>
       <c r="I49" s="4" t="s">
         <v>11</v>
@@ -3063,23 +3060,23 @@
         <v>49</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>150</v>
+        <v>134</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>304</v>
+        <v>283</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>305</v>
+        <v>284</v>
       </c>
       <c r="E50" s="4" t="s">
-        <v>306</v>
+        <v>285</v>
       </c>
       <c r="F50" s="4"/>
       <c r="G50" s="4" t="s">
-        <v>307</v>
+        <v>286</v>
       </c>
       <c r="H50" s="4" t="s">
-        <v>307</v>
+        <v>286</v>
       </c>
       <c r="I50" s="4" t="s">
         <v>11</v>
@@ -3090,23 +3087,23 @@
         <v>50</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>150</v>
+        <v>134</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>152</v>
+        <v>136</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>309</v>
+        <v>288</v>
       </c>
       <c r="E51" s="4" t="s">
-        <v>310</v>
+        <v>289</v>
       </c>
       <c r="F51" s="4"/>
       <c r="G51" s="4" t="s">
-        <v>151</v>
+        <v>135</v>
       </c>
       <c r="H51" s="4" t="s">
-        <v>151</v>
+        <v>135</v>
       </c>
       <c r="I51" s="4" t="s">
         <v>11</v>
@@ -3117,23 +3114,23 @@
         <v>51</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>150</v>
+        <v>134</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>308</v>
+        <v>287</v>
       </c>
       <c r="D52" s="4" t="s">
-        <v>311</v>
+        <v>290</v>
       </c>
       <c r="E52" s="4" t="s">
-        <v>312</v>
+        <v>291</v>
       </c>
       <c r="F52" s="4"/>
       <c r="G52" s="4" t="s">
-        <v>151</v>
+        <v>135</v>
       </c>
       <c r="H52" s="4" t="s">
-        <v>151</v>
+        <v>135</v>
       </c>
       <c r="I52" s="4" t="s">
         <v>11</v>
@@ -3144,23 +3141,23 @@
         <v>52</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>150</v>
+        <v>134</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>157</v>
+        <v>141</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>153</v>
+        <v>137</v>
       </c>
       <c r="E53" s="4" t="s">
-        <v>154</v>
+        <v>138</v>
       </c>
       <c r="F53" s="4"/>
       <c r="G53" s="4" t="s">
-        <v>155</v>
+        <v>139</v>
       </c>
       <c r="H53" s="4" t="s">
-        <v>156</v>
+        <v>140</v>
       </c>
       <c r="I53" s="4" t="s">
         <v>11</v>
@@ -3171,23 +3168,23 @@
         <v>53</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>150</v>
+        <v>134</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>158</v>
+        <v>142</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>153</v>
+        <v>137</v>
       </c>
       <c r="E54" s="4" t="s">
-        <v>159</v>
+        <v>143</v>
       </c>
       <c r="F54" s="4"/>
       <c r="G54" s="4" t="s">
-        <v>155</v>
+        <v>139</v>
       </c>
       <c r="H54" s="4" t="s">
-        <v>226</v>
+        <v>207</v>
       </c>
       <c r="I54" s="4" t="s">
         <v>11</v>
@@ -3198,23 +3195,23 @@
         <v>54</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>150</v>
+        <v>134</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>160</v>
+        <v>144</v>
       </c>
       <c r="D55" s="4" t="s">
-        <v>161</v>
+        <v>145</v>
       </c>
       <c r="E55" s="4" t="s">
-        <v>313</v>
+        <v>292</v>
       </c>
       <c r="F55" s="4"/>
       <c r="G55" s="4" t="s">
-        <v>162</v>
+        <v>146</v>
       </c>
       <c r="H55" s="4" t="s">
-        <v>163</v>
+        <v>147</v>
       </c>
       <c r="I55" s="4" t="s">
         <v>11</v>
@@ -3225,21 +3222,21 @@
         <v>55</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>150</v>
+        <v>134</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>318</v>
+        <v>297</v>
       </c>
       <c r="D56" s="4" t="s">
-        <v>319</v>
+        <v>298</v>
       </c>
       <c r="E56" s="4"/>
       <c r="F56" s="4"/>
       <c r="G56" s="4" t="s">
-        <v>320</v>
+        <v>299</v>
       </c>
       <c r="H56" s="4" t="s">
-        <v>320</v>
+        <v>299</v>
       </c>
       <c r="I56" s="4" t="s">
         <v>11</v>
@@ -3250,23 +3247,23 @@
         <v>56</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>166</v>
+        <v>150</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="D57" s="4" t="s">
-        <v>255</v>
+        <v>234</v>
       </c>
       <c r="E57" s="4" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="F57" s="4"/>
       <c r="G57" s="4" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="H57" s="4" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="I57" s="4" t="s">
         <v>11</v>
@@ -3277,23 +3274,23 @@
         <v>57</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>166</v>
+        <v>150</v>
       </c>
       <c r="C58" s="8" t="s">
-        <v>335</v>
+        <v>314</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>255</v>
+        <v>234</v>
       </c>
       <c r="E58" s="4" t="s">
-        <v>353</v>
+        <v>332</v>
       </c>
       <c r="F58" s="4"/>
       <c r="G58" s="4" t="s">
-        <v>167</v>
+        <v>151</v>
       </c>
       <c r="H58" s="4" t="s">
-        <v>167</v>
+        <v>151</v>
       </c>
       <c r="I58" s="4" t="s">
         <v>11</v>
@@ -3304,23 +3301,23 @@
         <v>58</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>166</v>
+        <v>150</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>168</v>
+        <v>152</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>255</v>
+        <v>234</v>
       </c>
       <c r="E59" s="4" t="s">
-        <v>352</v>
+        <v>331</v>
       </c>
       <c r="F59" s="4"/>
       <c r="G59" s="4" t="s">
-        <v>170</v>
+        <v>154</v>
       </c>
       <c r="H59" s="4" t="s">
-        <v>169</v>
+        <v>153</v>
       </c>
       <c r="I59" s="4" t="s">
         <v>11</v>
@@ -3331,23 +3328,23 @@
         <v>59</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="D60" s="4" t="s">
-        <v>255</v>
+        <v>234</v>
       </c>
       <c r="E60" s="4" t="s">
-        <v>289</v>
+        <v>268</v>
       </c>
       <c r="F60" s="4"/>
       <c r="G60" s="4" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="H60" s="4" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="I60" s="4" t="s">
         <v>11</v>
@@ -3358,23 +3355,23 @@
         <v>60</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>336</v>
+        <v>315</v>
       </c>
       <c r="D61" s="4" t="s">
-        <v>255</v>
+        <v>234</v>
       </c>
       <c r="E61" s="4" t="s">
-        <v>171</v>
+        <v>155</v>
       </c>
       <c r="F61" s="4"/>
       <c r="G61" s="4" t="s">
-        <v>172</v>
+        <v>156</v>
       </c>
       <c r="H61" s="4" t="s">
-        <v>172</v>
+        <v>156</v>
       </c>
       <c r="I61" s="4" t="s">
         <v>11</v>
@@ -3385,23 +3382,23 @@
         <v>61</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>334</v>
+        <v>313</v>
       </c>
       <c r="D62" s="4" t="s">
-        <v>255</v>
+        <v>234</v>
       </c>
       <c r="E62" s="4" t="s">
-        <v>351</v>
+        <v>330</v>
       </c>
       <c r="F62" s="4"/>
       <c r="G62" s="4" t="s">
-        <v>173</v>
+        <v>157</v>
       </c>
       <c r="H62" s="4" t="s">
-        <v>174</v>
+        <v>158</v>
       </c>
       <c r="I62" s="4" t="s">
         <v>11</v>
@@ -3412,23 +3409,23 @@
         <v>62</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>349</v>
+        <v>328</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>349</v>
+        <v>328</v>
       </c>
       <c r="D63" s="4" t="s">
-        <v>255</v>
+        <v>234</v>
       </c>
       <c r="E63" s="4" t="s">
-        <v>350</v>
+        <v>329</v>
       </c>
       <c r="F63" s="4"/>
       <c r="G63" s="4" t="s">
-        <v>354</v>
+        <v>333</v>
       </c>
       <c r="H63" s="4" t="s">
-        <v>354</v>
+        <v>333</v>
       </c>
       <c r="I63" s="4" t="s">
         <v>11</v>
@@ -3439,23 +3436,23 @@
         <v>63</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>347</v>
+        <v>326</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>282</v>
+        <v>261</v>
       </c>
       <c r="D64" s="4" t="s">
-        <v>255</v>
+        <v>234</v>
       </c>
       <c r="E64" s="4" t="s">
-        <v>291</v>
+        <v>270</v>
       </c>
       <c r="F64" s="4"/>
       <c r="G64" s="4" t="s">
-        <v>286</v>
+        <v>265</v>
       </c>
       <c r="H64" s="4" t="s">
-        <v>287</v>
+        <v>266</v>
       </c>
       <c r="I64" s="4" t="s">
         <v>11</v>
@@ -3466,23 +3463,23 @@
         <v>64</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>347</v>
+        <v>326</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>284</v>
+        <v>263</v>
       </c>
       <c r="D65" s="4" t="s">
-        <v>255</v>
+        <v>234</v>
       </c>
       <c r="E65" s="4" t="s">
-        <v>292</v>
+        <v>271</v>
       </c>
       <c r="F65" s="4"/>
       <c r="G65" s="4" t="s">
-        <v>285</v>
+        <v>264</v>
       </c>
       <c r="H65" s="4" t="s">
-        <v>285</v>
+        <v>264</v>
       </c>
       <c r="I65" s="4" t="s">
         <v>11</v>
@@ -3493,23 +3490,23 @@
         <v>65</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>347</v>
+        <v>326</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>283</v>
+        <v>262</v>
       </c>
       <c r="D66" s="4" t="s">
-        <v>255</v>
+        <v>234</v>
       </c>
       <c r="E66" s="4" t="s">
-        <v>293</v>
+        <v>272</v>
       </c>
       <c r="F66" s="4"/>
       <c r="G66" s="4" t="s">
-        <v>288</v>
+        <v>267</v>
       </c>
       <c r="H66" s="4" t="s">
-        <v>288</v>
+        <v>267</v>
       </c>
       <c r="I66" s="4" t="s">
         <v>11</v>
@@ -3520,25 +3517,25 @@
         <v>66</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>348</v>
+        <v>327</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>134</v>
+        <v>122</v>
       </c>
       <c r="D67" s="4" t="s">
-        <v>255</v>
+        <v>234</v>
       </c>
       <c r="E67" s="4" t="s">
-        <v>294</v>
+        <v>273</v>
       </c>
       <c r="F67" s="4" t="s">
-        <v>296</v>
+        <v>275</v>
       </c>
       <c r="G67" s="4" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="H67" s="4" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="I67" s="4" t="s">
         <v>11</v>
@@ -3549,19 +3546,19 @@
         <v>67</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>348</v>
+        <v>327</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>134</v>
+        <v>122</v>
       </c>
       <c r="D68" s="4" t="s">
-        <v>255</v>
+        <v>234</v>
       </c>
       <c r="E68" s="4" t="s">
-        <v>295</v>
+        <v>274</v>
       </c>
       <c r="F68" s="4" t="s">
-        <v>297</v>
+        <v>276</v>
       </c>
       <c r="G68" s="4" t="s">
         <v>10</v>
@@ -3578,25 +3575,25 @@
         <v>68</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>348</v>
+        <v>327</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>135</v>
+        <v>123</v>
       </c>
       <c r="D69" s="4" t="s">
-        <v>255</v>
+        <v>234</v>
       </c>
       <c r="E69" s="4" t="s">
-        <v>230</v>
+        <v>211</v>
       </c>
       <c r="F69" s="4" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
       <c r="G69" s="4" t="s">
-        <v>298</v>
+        <v>277</v>
       </c>
       <c r="H69" s="4" t="s">
-        <v>298</v>
+        <v>277</v>
       </c>
       <c r="I69" s="4" t="s">
         <v>11</v>
@@ -3607,25 +3604,25 @@
         <v>69</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>348</v>
+        <v>327</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>135</v>
+        <v>123</v>
       </c>
       <c r="D70" s="4" t="s">
-        <v>255</v>
+        <v>234</v>
       </c>
       <c r="E70" s="4" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="F70" s="4" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
       <c r="G70" s="4" t="s">
-        <v>143</v>
+        <v>354</v>
       </c>
       <c r="H70" s="4" t="s">
-        <v>143</v>
+        <v>354</v>
       </c>
       <c r="I70" s="4" t="s">
         <v>11</v>
@@ -3636,25 +3633,25 @@
         <v>70</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>348</v>
+        <v>327</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
       <c r="D71" s="4" t="s">
-        <v>255</v>
+        <v>234</v>
       </c>
       <c r="E71" s="4" t="s">
-        <v>299</v>
+        <v>278</v>
       </c>
       <c r="F71" s="4" t="s">
-        <v>144</v>
+        <v>131</v>
       </c>
       <c r="G71" s="4" t="s">
-        <v>145</v>
+        <v>353</v>
       </c>
       <c r="H71" s="4" t="s">
-        <v>145</v>
+        <v>353</v>
       </c>
       <c r="I71" s="4" t="s">
         <v>11</v>
@@ -3665,19 +3662,19 @@
         <v>71</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>348</v>
+        <v>327</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
       <c r="D72" s="4" t="s">
-        <v>255</v>
+        <v>234</v>
       </c>
       <c r="E72" s="4" t="s">
-        <v>300</v>
+        <v>279</v>
       </c>
       <c r="F72" s="4" t="s">
-        <v>302</v>
+        <v>281</v>
       </c>
       <c r="G72" s="4" t="s">
         <v>10</v>
@@ -3694,19 +3691,19 @@
         <v>72</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>348</v>
+        <v>327</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
       <c r="D73" s="4" t="s">
-        <v>255</v>
+        <v>234</v>
       </c>
       <c r="E73" s="4" t="s">
-        <v>301</v>
+        <v>280</v>
       </c>
       <c r="F73" s="4" t="s">
-        <v>303</v>
+        <v>282</v>
       </c>
       <c r="G73" s="4" t="s">
         <v>10</v>
@@ -3723,23 +3720,23 @@
         <v>73</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>348</v>
+        <v>327</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>137</v>
+        <v>125</v>
       </c>
       <c r="D74" s="4" t="s">
-        <v>255</v>
+        <v>234</v>
       </c>
       <c r="E74" s="4" t="s">
-        <v>148</v>
+        <v>132</v>
       </c>
       <c r="F74" s="4"/>
       <c r="G74" s="4" t="s">
-        <v>146</v>
+        <v>355</v>
       </c>
       <c r="H74" s="4" t="s">
-        <v>146</v>
+        <v>355</v>
       </c>
       <c r="I74" s="4" t="s">
         <v>11</v>
@@ -3750,23 +3747,23 @@
         <v>74</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>348</v>
+        <v>327</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="D75" s="4" t="s">
-        <v>255</v>
+        <v>234</v>
       </c>
       <c r="E75" s="4" t="s">
-        <v>149</v>
+        <v>133</v>
       </c>
       <c r="F75" s="4"/>
       <c r="G75" s="4" t="s">
-        <v>147</v>
+        <v>356</v>
       </c>
       <c r="H75" s="4" t="s">
-        <v>147</v>
+        <v>356</v>
       </c>
       <c r="I75" s="4" t="s">
         <v>11</v>
@@ -3777,23 +3774,23 @@
         <v>75</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>355</v>
+        <v>334</v>
       </c>
       <c r="C76" s="4" t="s">
-        <v>177</v>
+        <v>161</v>
       </c>
       <c r="D76" s="4" t="s">
-        <v>316</v>
+        <v>295</v>
       </c>
       <c r="E76" s="4" t="s">
-        <v>175</v>
+        <v>159</v>
       </c>
       <c r="F76" s="4"/>
       <c r="G76" s="4" t="s">
-        <v>176</v>
+        <v>160</v>
       </c>
       <c r="H76" s="4" t="s">
-        <v>176</v>
+        <v>160</v>
       </c>
       <c r="I76" s="4" t="s">
         <v>11</v>
@@ -3804,23 +3801,23 @@
         <v>76</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>355</v>
+        <v>334</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>178</v>
+        <v>162</v>
       </c>
       <c r="D77" s="4" t="s">
-        <v>317</v>
+        <v>296</v>
       </c>
       <c r="E77" s="4" t="s">
-        <v>175</v>
+        <v>159</v>
       </c>
       <c r="F77" s="4"/>
       <c r="G77" s="4" t="s">
-        <v>179</v>
+        <v>163</v>
       </c>
       <c r="H77" s="4" t="s">
-        <v>179</v>
+        <v>163</v>
       </c>
       <c r="I77" s="4" t="s">
         <v>11</v>
@@ -3831,23 +3828,23 @@
         <v>77</v>
       </c>
       <c r="B78" s="4" t="s">
-        <v>356</v>
+        <v>335</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>180</v>
+        <v>164</v>
       </c>
       <c r="D78" s="4" t="s">
-        <v>322</v>
+        <v>301</v>
       </c>
       <c r="E78" s="4" t="s">
-        <v>192</v>
+        <v>176</v>
       </c>
       <c r="F78" s="4"/>
       <c r="G78" s="4" t="s">
-        <v>181</v>
+        <v>165</v>
       </c>
       <c r="H78" s="4" t="s">
-        <v>181</v>
+        <v>165</v>
       </c>
       <c r="I78" s="4" t="s">
         <v>11</v>
@@ -3858,23 +3855,23 @@
         <v>78</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>356</v>
+        <v>335</v>
       </c>
       <c r="C79" s="4" t="s">
-        <v>182</v>
+        <v>166</v>
       </c>
       <c r="D79" s="4" t="s">
-        <v>322</v>
+        <v>301</v>
       </c>
       <c r="E79" s="4" t="s">
-        <v>193</v>
+        <v>177</v>
       </c>
       <c r="F79" s="4"/>
       <c r="G79" s="4" t="s">
-        <v>185</v>
+        <v>169</v>
       </c>
       <c r="H79" s="4" t="s">
-        <v>185</v>
+        <v>169</v>
       </c>
       <c r="I79" s="4" t="s">
         <v>11</v>
@@ -3885,23 +3882,23 @@
         <v>79</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>356</v>
+        <v>335</v>
       </c>
       <c r="C80" s="4" t="s">
-        <v>183</v>
+        <v>167</v>
       </c>
       <c r="D80" s="4" t="s">
-        <v>322</v>
+        <v>301</v>
       </c>
       <c r="E80" s="4" t="s">
-        <v>194</v>
+        <v>178</v>
       </c>
       <c r="F80" s="4"/>
       <c r="G80" s="4" t="s">
-        <v>186</v>
+        <v>170</v>
       </c>
       <c r="H80" s="4" t="s">
-        <v>186</v>
+        <v>170</v>
       </c>
       <c r="I80" s="4" t="s">
         <v>11</v>
@@ -3912,23 +3909,23 @@
         <v>80</v>
       </c>
       <c r="B81" s="4" t="s">
-        <v>356</v>
+        <v>335</v>
       </c>
       <c r="C81" s="4" t="s">
-        <v>184</v>
+        <v>168</v>
       </c>
       <c r="D81" s="4" t="s">
-        <v>322</v>
+        <v>301</v>
       </c>
       <c r="E81" s="4" t="s">
-        <v>195</v>
+        <v>179</v>
       </c>
       <c r="F81" s="4"/>
       <c r="G81" s="4" t="s">
-        <v>187</v>
+        <v>171</v>
       </c>
       <c r="H81" s="4" t="s">
-        <v>187</v>
+        <v>171</v>
       </c>
       <c r="I81" s="4" t="s">
         <v>11</v>
@@ -3939,20 +3936,20 @@
         <v>81</v>
       </c>
       <c r="B82" s="4" t="s">
-        <v>356</v>
+        <v>335</v>
       </c>
       <c r="C82" s="4" t="s">
-        <v>188</v>
+        <v>172</v>
       </c>
       <c r="D82" s="4" t="s">
-        <v>322</v>
+        <v>301</v>
       </c>
       <c r="E82" s="4" t="s">
-        <v>196</v>
+        <v>180</v>
       </c>
       <c r="F82" s="4"/>
       <c r="G82" s="4" t="s">
-        <v>200</v>
+        <v>184</v>
       </c>
       <c r="H82" s="4"/>
       <c r="I82" s="4" t="s">
@@ -3964,23 +3961,23 @@
         <v>82</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>356</v>
+        <v>335</v>
       </c>
       <c r="C83" s="4" t="s">
-        <v>189</v>
+        <v>173</v>
       </c>
       <c r="D83" s="4" t="s">
-        <v>322</v>
+        <v>301</v>
       </c>
       <c r="E83" s="4" t="s">
-        <v>197</v>
+        <v>181</v>
       </c>
       <c r="F83" s="4"/>
       <c r="G83" s="4" t="s">
-        <v>201</v>
+        <v>185</v>
       </c>
       <c r="H83" s="4" t="s">
-        <v>201</v>
+        <v>185</v>
       </c>
       <c r="I83" s="4" t="s">
         <v>11</v>
@@ -3991,23 +3988,23 @@
         <v>83</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>356</v>
+        <v>335</v>
       </c>
       <c r="C84" s="4" t="s">
-        <v>190</v>
+        <v>174</v>
       </c>
       <c r="D84" s="4" t="s">
-        <v>322</v>
+        <v>301</v>
       </c>
       <c r="E84" s="4" t="s">
-        <v>198</v>
+        <v>182</v>
       </c>
       <c r="F84" s="4"/>
       <c r="G84" s="4" t="s">
-        <v>202</v>
+        <v>186</v>
       </c>
       <c r="H84" s="4" t="s">
-        <v>202</v>
+        <v>186</v>
       </c>
       <c r="I84" s="4" t="s">
         <v>11</v>
@@ -4018,23 +4015,23 @@
         <v>84</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>356</v>
+        <v>335</v>
       </c>
       <c r="C85" s="4" t="s">
-        <v>191</v>
+        <v>175</v>
       </c>
       <c r="D85" s="4" t="s">
-        <v>322</v>
+        <v>301</v>
       </c>
       <c r="E85" s="4" t="s">
-        <v>199</v>
+        <v>183</v>
       </c>
       <c r="F85" s="4"/>
       <c r="G85" s="4" t="s">
-        <v>203</v>
+        <v>187</v>
       </c>
       <c r="H85" s="4" t="s">
-        <v>203</v>
+        <v>187</v>
       </c>
       <c r="I85" s="4" t="s">
         <v>11</v>
@@ -4045,23 +4042,23 @@
         <v>85</v>
       </c>
       <c r="B86" s="4" t="s">
-        <v>356</v>
+        <v>335</v>
       </c>
       <c r="C86" s="4" t="s">
-        <v>204</v>
+        <v>188</v>
       </c>
       <c r="D86" s="4" t="s">
-        <v>322</v>
+        <v>301</v>
       </c>
       <c r="E86" s="4" t="s">
-        <v>209</v>
+        <v>193</v>
       </c>
       <c r="F86" s="4"/>
       <c r="G86" s="4" t="s">
-        <v>214</v>
+        <v>198</v>
       </c>
       <c r="H86" s="4" t="s">
-        <v>214</v>
+        <v>198</v>
       </c>
       <c r="I86" s="4" t="s">
         <v>11</v>
@@ -4072,23 +4069,23 @@
         <v>86</v>
       </c>
       <c r="B87" s="4" t="s">
-        <v>356</v>
+        <v>335</v>
       </c>
       <c r="C87" s="4" t="s">
-        <v>205</v>
+        <v>189</v>
       </c>
       <c r="D87" s="4" t="s">
-        <v>322</v>
+        <v>301</v>
       </c>
       <c r="E87" s="4" t="s">
-        <v>210</v>
+        <v>194</v>
       </c>
       <c r="F87" s="4"/>
       <c r="G87" s="4" t="s">
-        <v>215</v>
+        <v>199</v>
       </c>
       <c r="H87" s="4" t="s">
-        <v>215</v>
+        <v>199</v>
       </c>
       <c r="I87" s="4" t="s">
         <v>11</v>
@@ -4099,23 +4096,23 @@
         <v>87</v>
       </c>
       <c r="B88" s="4" t="s">
-        <v>356</v>
+        <v>335</v>
       </c>
       <c r="C88" s="4" t="s">
-        <v>206</v>
+        <v>190</v>
       </c>
       <c r="D88" s="4" t="s">
-        <v>322</v>
+        <v>301</v>
       </c>
       <c r="E88" s="4" t="s">
-        <v>211</v>
+        <v>195</v>
       </c>
       <c r="F88" s="4"/>
       <c r="G88" s="4" t="s">
-        <v>215</v>
+        <v>199</v>
       </c>
       <c r="H88" s="4" t="s">
-        <v>215</v>
+        <v>199</v>
       </c>
       <c r="I88" s="4" t="s">
         <v>11</v>
@@ -4126,23 +4123,23 @@
         <v>88</v>
       </c>
       <c r="B89" s="4" t="s">
-        <v>356</v>
+        <v>335</v>
       </c>
       <c r="C89" s="4" t="s">
-        <v>207</v>
+        <v>191</v>
       </c>
       <c r="D89" s="4" t="s">
-        <v>322</v>
+        <v>301</v>
       </c>
       <c r="E89" s="4" t="s">
-        <v>212</v>
+        <v>196</v>
       </c>
       <c r="F89" s="4"/>
       <c r="G89" s="4" t="s">
-        <v>215</v>
+        <v>199</v>
       </c>
       <c r="H89" s="4" t="s">
-        <v>215</v>
+        <v>199</v>
       </c>
       <c r="I89" s="4" t="s">
         <v>11</v>
@@ -4153,23 +4150,23 @@
         <v>89</v>
       </c>
       <c r="B90" s="4" t="s">
-        <v>356</v>
+        <v>335</v>
       </c>
       <c r="C90" s="4" t="s">
-        <v>208</v>
+        <v>192</v>
       </c>
       <c r="D90" s="4" t="s">
-        <v>322</v>
+        <v>301</v>
       </c>
       <c r="E90" s="4" t="s">
-        <v>213</v>
+        <v>197</v>
       </c>
       <c r="F90" s="4"/>
       <c r="G90" s="4" t="s">
-        <v>215</v>
+        <v>199</v>
       </c>
       <c r="H90" s="4" t="s">
-        <v>215</v>
+        <v>199</v>
       </c>
       <c r="I90" s="4" t="s">
         <v>11</v>
@@ -4180,23 +4177,23 @@
         <v>90</v>
       </c>
       <c r="B91" s="4" t="s">
-        <v>356</v>
+        <v>335</v>
       </c>
       <c r="C91" s="4" t="s">
-        <v>216</v>
+        <v>200</v>
       </c>
       <c r="D91" s="4" t="s">
-        <v>322</v>
+        <v>301</v>
       </c>
       <c r="E91" s="4" t="s">
-        <v>217</v>
+        <v>201</v>
       </c>
       <c r="F91" s="4"/>
       <c r="G91" s="4" t="s">
-        <v>218</v>
+        <v>202</v>
       </c>
       <c r="H91" s="4" t="s">
-        <v>218</v>
+        <v>202</v>
       </c>
       <c r="I91" s="4" t="s">
         <v>11</v>
@@ -4207,23 +4204,23 @@
         <v>91</v>
       </c>
       <c r="B92" s="4" t="s">
-        <v>219</v>
+        <v>203</v>
       </c>
       <c r="C92" s="4" t="s">
-        <v>337</v>
+        <v>316</v>
       </c>
       <c r="D92" s="4" t="s">
-        <v>322</v>
+        <v>301</v>
       </c>
       <c r="E92" s="4" t="s">
-        <v>221</v>
+        <v>205</v>
       </c>
       <c r="F92" s="4"/>
       <c r="G92" s="4" t="s">
-        <v>222</v>
+        <v>358</v>
       </c>
       <c r="H92" s="4" t="s">
-        <v>222</v>
+        <v>358</v>
       </c>
       <c r="I92" s="4" t="s">
         <v>11</v>
@@ -4234,23 +4231,23 @@
         <v>92</v>
       </c>
       <c r="B93" s="4" t="s">
-        <v>219</v>
+        <v>203</v>
       </c>
       <c r="C93" s="4" t="s">
-        <v>338</v>
+        <v>317</v>
       </c>
       <c r="D93" s="4" t="s">
-        <v>322</v>
+        <v>301</v>
       </c>
       <c r="E93" s="4" t="s">
-        <v>220</v>
+        <v>204</v>
       </c>
       <c r="F93" s="4"/>
       <c r="G93" s="4" t="s">
-        <v>223</v>
+        <v>357</v>
       </c>
       <c r="H93" s="4" t="s">
-        <v>223</v>
+        <v>357</v>
       </c>
       <c r="I93" s="4" t="s">
         <v>11</v>
@@ -4261,23 +4258,23 @@
         <v>93</v>
       </c>
       <c r="B94" s="4" t="s">
-        <v>219</v>
+        <v>203</v>
       </c>
       <c r="C94" s="4" t="s">
-        <v>325</v>
+        <v>304</v>
       </c>
       <c r="D94" s="4" t="s">
-        <v>322</v>
+        <v>301</v>
       </c>
       <c r="E94" s="4" t="s">
-        <v>327</v>
+        <v>306</v>
       </c>
       <c r="F94" s="4"/>
       <c r="G94" s="4" t="s">
-        <v>330</v>
+        <v>309</v>
       </c>
       <c r="H94" s="4" t="s">
-        <v>330</v>
+        <v>309</v>
       </c>
       <c r="I94" s="4" t="s">
         <v>11</v>
@@ -4288,23 +4285,23 @@
         <v>94</v>
       </c>
       <c r="B95" s="4" t="s">
-        <v>219</v>
+        <v>203</v>
       </c>
       <c r="C95" s="4" t="s">
-        <v>326</v>
+        <v>305</v>
       </c>
       <c r="D95" s="4" t="s">
-        <v>322</v>
+        <v>301</v>
       </c>
       <c r="E95" s="4" t="s">
-        <v>328</v>
+        <v>307</v>
       </c>
       <c r="F95" s="4"/>
       <c r="G95" s="4" t="s">
-        <v>329</v>
+        <v>308</v>
       </c>
       <c r="H95" s="4" t="s">
-        <v>329</v>
+        <v>308</v>
       </c>
       <c r="I95" s="4" t="s">
         <v>11</v>
@@ -4315,23 +4312,23 @@
         <v>95</v>
       </c>
       <c r="B96" s="4" t="s">
-        <v>219</v>
+        <v>203</v>
       </c>
       <c r="C96" s="4" t="s">
-        <v>339</v>
+        <v>318</v>
       </c>
       <c r="D96" s="4" t="s">
-        <v>153</v>
+        <v>137</v>
       </c>
       <c r="E96" s="4" t="s">
-        <v>231</v>
+        <v>212</v>
       </c>
       <c r="F96" s="4"/>
       <c r="G96" s="4" t="s">
-        <v>232</v>
+        <v>213</v>
       </c>
       <c r="H96" s="4" t="s">
-        <v>232</v>
+        <v>213</v>
       </c>
       <c r="I96" s="4" t="s">
         <v>11</v>
@@ -4342,23 +4339,23 @@
         <v>96</v>
       </c>
       <c r="B97" s="4" t="s">
-        <v>219</v>
+        <v>203</v>
       </c>
       <c r="C97" s="4" t="s">
-        <v>340</v>
+        <v>319</v>
       </c>
       <c r="D97" s="4" t="s">
-        <v>153</v>
+        <v>137</v>
       </c>
       <c r="E97" s="4" t="s">
-        <v>343</v>
+        <v>322</v>
       </c>
       <c r="F97" s="4"/>
       <c r="G97" s="4" t="s">
-        <v>233</v>
+        <v>359</v>
       </c>
       <c r="H97" s="4" t="s">
-        <v>233</v>
+        <v>359</v>
       </c>
       <c r="I97" s="4" t="s">
         <v>11</v>
@@ -4369,23 +4366,23 @@
         <v>97</v>
       </c>
       <c r="B98" s="4" t="s">
-        <v>219</v>
+        <v>203</v>
       </c>
       <c r="C98" s="4" t="s">
-        <v>341</v>
+        <v>320</v>
       </c>
       <c r="D98" s="4" t="s">
-        <v>153</v>
+        <v>137</v>
       </c>
       <c r="E98" s="4" t="s">
-        <v>342</v>
+        <v>321</v>
       </c>
       <c r="F98" s="4"/>
       <c r="G98" s="4" t="s">
-        <v>233</v>
+        <v>359</v>
       </c>
       <c r="H98" s="4" t="s">
-        <v>233</v>
+        <v>359</v>
       </c>
       <c r="I98" s="4" t="s">
         <v>11</v>
@@ -4396,23 +4393,23 @@
         <v>98</v>
       </c>
       <c r="B99" s="4" t="s">
-        <v>224</v>
+        <v>206</v>
       </c>
       <c r="C99" s="4" t="s">
-        <v>331</v>
+        <v>310</v>
       </c>
       <c r="D99" s="4" t="s">
-        <v>322</v>
+        <v>301</v>
       </c>
       <c r="E99" s="4" t="s">
-        <v>357</v>
+        <v>336</v>
       </c>
       <c r="F99" s="4"/>
       <c r="G99" s="4" t="s">
-        <v>321</v>
+        <v>300</v>
       </c>
       <c r="H99" s="4" t="s">
-        <v>321</v>
+        <v>300</v>
       </c>
       <c r="I99" s="4" t="s">
         <v>11</v>
@@ -4423,23 +4420,23 @@
         <v>99</v>
       </c>
       <c r="B100" s="4" t="s">
-        <v>234</v>
+        <v>214</v>
       </c>
       <c r="C100" s="4" t="s">
-        <v>332</v>
+        <v>311</v>
       </c>
       <c r="D100" s="4" t="s">
-        <v>322</v>
+        <v>301</v>
       </c>
       <c r="E100" s="4" t="s">
-        <v>358</v>
+        <v>337</v>
       </c>
       <c r="F100" s="4"/>
       <c r="G100" s="4" t="s">
-        <v>225</v>
+        <v>300</v>
       </c>
       <c r="H100" s="4" t="s">
-        <v>225</v>
+        <v>300</v>
       </c>
       <c r="I100" s="4" t="s">
         <v>11</v>
@@ -4450,23 +4447,23 @@
         <v>100</v>
       </c>
       <c r="B101" s="4" t="s">
-        <v>234</v>
+        <v>214</v>
       </c>
       <c r="C101" s="4" t="s">
-        <v>333</v>
+        <v>312</v>
       </c>
       <c r="D101" s="4" t="s">
-        <v>322</v>
+        <v>301</v>
       </c>
       <c r="E101" s="4" t="s">
-        <v>359</v>
+        <v>338</v>
       </c>
       <c r="F101" s="4"/>
       <c r="G101" s="4" t="s">
-        <v>225</v>
+        <v>300</v>
       </c>
       <c r="H101" s="4" t="s">
-        <v>225</v>
+        <v>300</v>
       </c>
       <c r="I101" s="4" t="s">
         <v>11</v>
@@ -4477,23 +4474,23 @@
         <v>101</v>
       </c>
       <c r="B102" s="4" t="s">
-        <v>234</v>
+        <v>214</v>
       </c>
       <c r="C102" s="4" t="s">
-        <v>360</v>
+        <v>339</v>
       </c>
       <c r="D102" s="4" t="s">
-        <v>322</v>
+        <v>301</v>
       </c>
       <c r="E102" s="4" t="s">
-        <v>324</v>
+        <v>303</v>
       </c>
       <c r="F102" s="4"/>
       <c r="G102" s="4" t="s">
-        <v>227</v>
+        <v>208</v>
       </c>
       <c r="H102" s="4" t="s">
-        <v>227</v>
+        <v>208</v>
       </c>
       <c r="I102" s="4" t="s">
         <v>11</v>
@@ -4504,23 +4501,23 @@
         <v>102</v>
       </c>
       <c r="B103" s="4" t="s">
-        <v>234</v>
+        <v>214</v>
       </c>
       <c r="C103" s="4" t="s">
-        <v>361</v>
+        <v>340</v>
       </c>
       <c r="D103" s="4" t="s">
-        <v>322</v>
+        <v>301</v>
       </c>
       <c r="E103" s="4" t="s">
-        <v>323</v>
+        <v>302</v>
       </c>
       <c r="F103" s="4"/>
       <c r="G103" s="4" t="s">
-        <v>228</v>
+        <v>209</v>
       </c>
       <c r="H103" s="4" t="s">
-        <v>229</v>
+        <v>210</v>
       </c>
       <c r="I103" s="4" t="s">
         <v>11</v>
@@ -4531,23 +4528,23 @@
         <v>103</v>
       </c>
       <c r="B104" s="4" t="s">
-        <v>235</v>
+        <v>215</v>
       </c>
       <c r="C104" s="4" t="s">
-        <v>237</v>
+        <v>217</v>
       </c>
       <c r="D104" s="4" t="s">
-        <v>322</v>
+        <v>301</v>
       </c>
       <c r="E104" s="4" t="s">
-        <v>238</v>
+        <v>360</v>
       </c>
       <c r="F104" s="4"/>
       <c r="G104" s="4" t="s">
-        <v>236</v>
+        <v>216</v>
       </c>
       <c r="H104" s="4" t="s">
-        <v>236</v>
+        <v>216</v>
       </c>
       <c r="I104" s="4" t="s">
         <v>11</v>
@@ -4558,23 +4555,23 @@
         <v>104</v>
       </c>
       <c r="B105" s="4" t="s">
-        <v>235</v>
+        <v>215</v>
       </c>
       <c r="C105" s="4" t="s">
-        <v>239</v>
+        <v>218</v>
       </c>
       <c r="D105" s="4" t="s">
-        <v>322</v>
+        <v>301</v>
       </c>
       <c r="E105" s="4" t="s">
-        <v>240</v>
+        <v>219</v>
       </c>
       <c r="F105" s="4"/>
       <c r="G105" s="4" t="s">
-        <v>236</v>
+        <v>216</v>
       </c>
       <c r="H105" s="4" t="s">
-        <v>236</v>
+        <v>216</v>
       </c>
       <c r="I105" s="4" t="s">
         <v>11</v>

</xml_diff>